<commit_message>
Update of the testing menu for LLPDisplacedJets
</commit_message>
<xml_diff>
--- a/development/L1Menu_LLPDisplacedJets_test_v2/PrescaleTable/L1Menu_LLPDisplacedJets_test_v2.xlsx
+++ b/development/L1Menu_LLPDisplacedJets_test_v2/PrescaleTable/L1Menu_LLPDisplacedJets_test_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_LLPDisplacedJets_test_v2/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A771BF86-1BB7-454B-852E-EDAA0D801EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625E9C12-6FB2-C44F-9FA8-7F6BB40CD9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>L1_SingleJet50er2p9</t>
+  </si>
+  <si>
+    <t>L1_HTT120_SingleLLPJet40</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -925,6 +928,41 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>